<commit_message>
eBird filtered on MARC accepts list
.fmw file filters ebird dataset by species in marc accept list, also added a header to accept list bc idk how to fix the problem that occurs without it
</commit_message>
<xml_diff>
--- a/MARC_eBird_accept_species.xlsx
+++ b/MARC_eBird_accept_species.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Documents\school\ECO697\project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucyr\Documents\Databases\FinalProject697\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{343400CC-EEDD-433B-96EB-94814FEA256E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
   <si>
     <t>Black-bellied Whistling-Duck (eB)</t>
   </si>
@@ -186,12 +187,15 @@
   </si>
   <si>
     <t>Painted Bunting (eB)</t>
+  </si>
+  <si>
+    <t>Species</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -522,343 +526,346 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A54"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:A55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A21" s="2" t="s">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A22" s="2" t="s">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A23" s="2" t="s">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A24" s="2" t="s">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A25" s="2" t="s">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A26" s="2" t="s">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A27" s="2" t="s">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A28" s="2" t="s">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A29" s="2" t="s">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A30" s="2" t="s">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A31" s="2" t="s">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A32" s="2" t="s">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A33" s="2" t="s">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A34" s="2" t="s">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A35" s="2" t="s">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A36" s="2" t="s">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A37" s="2" t="s">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A38" s="2" t="s">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A39" s="2" t="s">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A40" s="2" t="s">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A41" s="2" t="s">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A42" s="2" t="s">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A43" s="2" t="s">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A44" s="2" t="s">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A45" s="2" t="s">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A46" s="2" t="s">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A47" s="2" t="s">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A48" s="2" t="s">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A49" s="1" t="s">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A50" s="2" t="s">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A51" s="2" t="s">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A52" s="2" t="s">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A53" s="2" t="s">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A54" s="2" t="s">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" s="2" t="s">
         <v>53</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" display="http://www.maavianrecords.com/review-list/black-bellied-whistling-duck"/>
-    <hyperlink ref="A2" r:id="rId2" display="http://www.maavianrecords.com/review-list/pink-footed-goose"/>
-    <hyperlink ref="A3" r:id="rId3" display="http://www.maavianrecords.com/review-list/barnacle-goose"/>
-    <hyperlink ref="A4" r:id="rId4" display="http://www.maavianrecords.com/review-list/tundra-swan"/>
-    <hyperlink ref="A5" r:id="rId5" display="http://www.maavianrecords.com/review-list/tufted-duck"/>
-    <hyperlink ref="A6" r:id="rId6" display="http://www.maavianrecords.com/review-list/eared-grebe"/>
-    <hyperlink ref="A7" r:id="rId7" display="http://www.maavianrecords.com/review-list/white-winged-dove"/>
-    <hyperlink ref="A8" r:id="rId8" display="http://www.maavianrecords.com/review-list/rufous-hummingbird"/>
-    <hyperlink ref="A9" r:id="rId9" display="http://www.maavianrecords.com/review-list/yellow-rail"/>
-    <hyperlink ref="A10" r:id="rId10" display="http://www.maavianrecords.com/review-list/purple-gallinule"/>
-    <hyperlink ref="A11" r:id="rId11" display="http://www.maavianrecords.com/review-list/northern-lapwing"/>
-    <hyperlink ref="A12" r:id="rId12" display="http://www.maavianrecords.com/review-list/wilsons-plover"/>
-    <hyperlink ref="A13" r:id="rId13" display="http://www.maavianrecords.com/review-list/bar-tailed-godwit"/>
-    <hyperlink ref="A14" r:id="rId14" display="http://www.maavianrecords.com/review-list/ruff"/>
-    <hyperlink ref="A15" r:id="rId15" display="http://www.maavianrecords.com/review-list/curlew-sandpiper"/>
-    <hyperlink ref="A16" r:id="rId16" display="http://www.maavianrecords.com/review-list/great-skua"/>
-    <hyperlink ref="A17" r:id="rId17" display="http://www.maavianrecords.com/review-list/south-polar-skua"/>
-    <hyperlink ref="A18" r:id="rId18" display="http://www.maavianrecords.com/review-list/ivory-gull"/>
-    <hyperlink ref="A19" r:id="rId19" display="http://www.maavianrecords.com/review-list/franklins-gull"/>
-    <hyperlink ref="A20" r:id="rId20" display="http://www.maavianrecords.com/review-list/mew-gull"/>
-    <hyperlink ref="A21" r:id="rId21" display="http://www.maavianrecords.com/review-list/sooty-tern"/>
-    <hyperlink ref="A22" r:id="rId22" display="http://www.maavianrecords.com/review-list/bridled-tern"/>
-    <hyperlink ref="A23" r:id="rId23" display="http://www.maavianrecords.com/review-list/gull-billed-tern"/>
-    <hyperlink ref="A24" r:id="rId24" display="http://www.maavianrecords.com/review-list/pacific-loon"/>
-    <hyperlink ref="A25" r:id="rId25" display="http://www.maavianrecords.com/review-list/brown-booby"/>
-    <hyperlink ref="A26" r:id="rId26" display="http://www.maavianrecords.com/review-list/american-white-pelican"/>
-    <hyperlink ref="A27" r:id="rId27" display="http://www.maavianrecords.com/review-list/brown-pelican"/>
-    <hyperlink ref="A28" r:id="rId28" display="http://www.maavianrecords.com/review-list/white-ibis"/>
-    <hyperlink ref="A29" r:id="rId29" display="http://www.maavianrecords.com/review-list/white-faced-ibis"/>
-    <hyperlink ref="A30" r:id="rId30" display="http://www.maavianrecords.com/review-list/swallow-tailed-kite"/>
-    <hyperlink ref="A31" r:id="rId31" display="http://www.maavianrecords.com/review-list/white-tailed-kite"/>
-    <hyperlink ref="A32" r:id="rId32" display="http://www.maavianrecords.com/review-list/mississippi-kite"/>
-    <hyperlink ref="A33" r:id="rId33" display="http://www.maavianrecords.com/review-list/black-backed-woodpecker"/>
-    <hyperlink ref="A34" r:id="rId34" display="http://www.maavianrecords.com/review-list/says-phoebe"/>
-    <hyperlink ref="A35" r:id="rId35" display="http://www.maavianrecords.com/review-list/ash-throated-flycatcher"/>
-    <hyperlink ref="A36" r:id="rId36" display="http://www.maavianrecords.com/review-list/scissor-tailed-flycatcher"/>
-    <hyperlink ref="A37" r:id="rId37" display="http://www.maavianrecords.com/review-list/fork-tailed-flycatcher"/>
-    <hyperlink ref="A38" r:id="rId38" display="http://www.maavianrecords.com/review-list/loggerhead-shrike"/>
-    <hyperlink ref="A39" r:id="rId39" display="http://www.maavianrecords.com/review-list/bells-vireo"/>
-    <hyperlink ref="A40" r:id="rId40" display="http://www.maavianrecords.com/review-list/cave-swallow"/>
-    <hyperlink ref="A41" r:id="rId41" display="http://www.maavianrecords.com/review-list/boreal-chickadee"/>
-    <hyperlink ref="A42" r:id="rId42" display="http://www.maavianrecords.com/review-list/northern-wheatear"/>
-    <hyperlink ref="A43" r:id="rId43" display="http://www.maavianrecords.com/review-list/mountain-bluebird"/>
-    <hyperlink ref="A44" r:id="rId44" display="http://www.maavianrecords.com/review-list/townsends-solitaire"/>
-    <hyperlink ref="A45" r:id="rId45" display="http://www.maavianrecords.com/review-list/varied-thrush"/>
-    <hyperlink ref="A46" r:id="rId46" display="http://www.maavianrecords.com/review-list/black-throated-gray-warbler"/>
-    <hyperlink ref="A47" r:id="rId47" display="http://www.maavianrecords.com/review-list/townsends-warbler"/>
-    <hyperlink ref="A48" r:id="rId48" display="http://www.maavianrecords.com/review-list/green-tailed-towhee"/>
-    <hyperlink ref="A50" r:id="rId49" display="http://www.maavianrecords.com/review-list/le-contes-sparrow"/>
-    <hyperlink ref="A51" r:id="rId50" display="http://www.maavianrecords.com/review-list/harriss-sparrow"/>
-    <hyperlink ref="A52" r:id="rId51" display="http://www.maavianrecords.com/review-list/western-tanager"/>
-    <hyperlink ref="A53" r:id="rId52" display="http://www.maavianrecords.com/review-list/black-headed-grosbeak"/>
-    <hyperlink ref="A54" r:id="rId53" display="http://www.maavianrecords.com/review-list/painted-bunting"/>
+    <hyperlink ref="A2" r:id="rId1" display="http://www.maavianrecords.com/review-list/black-bellied-whistling-duck" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="A3" r:id="rId2" display="http://www.maavianrecords.com/review-list/pink-footed-goose" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="A4" r:id="rId3" display="http://www.maavianrecords.com/review-list/barnacle-goose" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="A5" r:id="rId4" display="http://www.maavianrecords.com/review-list/tundra-swan" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="A6" r:id="rId5" display="http://www.maavianrecords.com/review-list/tufted-duck" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="A7" r:id="rId6" display="http://www.maavianrecords.com/review-list/eared-grebe" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="A8" r:id="rId7" display="http://www.maavianrecords.com/review-list/white-winged-dove" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="A9" r:id="rId8" display="http://www.maavianrecords.com/review-list/rufous-hummingbird" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="A10" r:id="rId9" display="http://www.maavianrecords.com/review-list/yellow-rail" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="A11" r:id="rId10" display="http://www.maavianrecords.com/review-list/purple-gallinule" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="A12" r:id="rId11" display="http://www.maavianrecords.com/review-list/northern-lapwing" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="A13" r:id="rId12" display="http://www.maavianrecords.com/review-list/wilsons-plover" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="A14" r:id="rId13" display="http://www.maavianrecords.com/review-list/bar-tailed-godwit" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="A15" r:id="rId14" display="http://www.maavianrecords.com/review-list/ruff" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="A16" r:id="rId15" display="http://www.maavianrecords.com/review-list/curlew-sandpiper" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="A17" r:id="rId16" display="http://www.maavianrecords.com/review-list/great-skua" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="A18" r:id="rId17" display="http://www.maavianrecords.com/review-list/south-polar-skua" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="A19" r:id="rId18" display="http://www.maavianrecords.com/review-list/ivory-gull" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="A20" r:id="rId19" display="http://www.maavianrecords.com/review-list/franklins-gull" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="A21" r:id="rId20" display="http://www.maavianrecords.com/review-list/mew-gull" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="A22" r:id="rId21" display="http://www.maavianrecords.com/review-list/sooty-tern" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="A23" r:id="rId22" display="http://www.maavianrecords.com/review-list/bridled-tern" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="A24" r:id="rId23" display="http://www.maavianrecords.com/review-list/gull-billed-tern" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="A25" r:id="rId24" display="http://www.maavianrecords.com/review-list/pacific-loon" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="A26" r:id="rId25" display="http://www.maavianrecords.com/review-list/brown-booby" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="A27" r:id="rId26" display="http://www.maavianrecords.com/review-list/american-white-pelican" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="A28" r:id="rId27" display="http://www.maavianrecords.com/review-list/brown-pelican" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="A29" r:id="rId28" display="http://www.maavianrecords.com/review-list/white-ibis" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="A30" r:id="rId29" display="http://www.maavianrecords.com/review-list/white-faced-ibis" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="A31" r:id="rId30" display="http://www.maavianrecords.com/review-list/swallow-tailed-kite" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="A32" r:id="rId31" display="http://www.maavianrecords.com/review-list/white-tailed-kite" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="A33" r:id="rId32" display="http://www.maavianrecords.com/review-list/mississippi-kite" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="A34" r:id="rId33" display="http://www.maavianrecords.com/review-list/black-backed-woodpecker" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="A35" r:id="rId34" display="http://www.maavianrecords.com/review-list/says-phoebe" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="A36" r:id="rId35" display="http://www.maavianrecords.com/review-list/ash-throated-flycatcher" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="A37" r:id="rId36" display="http://www.maavianrecords.com/review-list/scissor-tailed-flycatcher" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="A38" r:id="rId37" display="http://www.maavianrecords.com/review-list/fork-tailed-flycatcher" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="A39" r:id="rId38" display="http://www.maavianrecords.com/review-list/loggerhead-shrike" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="A40" r:id="rId39" display="http://www.maavianrecords.com/review-list/bells-vireo" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="A41" r:id="rId40" display="http://www.maavianrecords.com/review-list/cave-swallow" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="A42" r:id="rId41" display="http://www.maavianrecords.com/review-list/boreal-chickadee" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="A43" r:id="rId42" display="http://www.maavianrecords.com/review-list/northern-wheatear" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="A44" r:id="rId43" display="http://www.maavianrecords.com/review-list/mountain-bluebird" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="A45" r:id="rId44" display="http://www.maavianrecords.com/review-list/townsends-solitaire" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="A46" r:id="rId45" display="http://www.maavianrecords.com/review-list/varied-thrush" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="A47" r:id="rId46" display="http://www.maavianrecords.com/review-list/black-throated-gray-warbler" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="A48" r:id="rId47" display="http://www.maavianrecords.com/review-list/townsends-warbler" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="A49" r:id="rId48" display="http://www.maavianrecords.com/review-list/green-tailed-towhee" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink ref="A51" r:id="rId49" display="http://www.maavianrecords.com/review-list/le-contes-sparrow" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
+    <hyperlink ref="A52" r:id="rId50" display="http://www.maavianrecords.com/review-list/harriss-sparrow" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
+    <hyperlink ref="A53" r:id="rId51" display="http://www.maavianrecords.com/review-list/western-tanager" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
+    <hyperlink ref="A54" r:id="rId52" display="http://www.maavianrecords.com/review-list/black-headed-grosbeak" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
+    <hyperlink ref="A55" r:id="rId53" display="http://www.maavianrecords.com/review-list/painted-bunting" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId54"/>

</xml_diff>